<commit_message>
Se programa la funcionalidad de cartera enmora y se hacen ajustes de interfaz.
</commit_message>
<xml_diff>
--- a/Tier.Services/PlantillasReportes/Cotizacion.xlsx
+++ b/Tier.Services/PlantillasReportes/Cotizacion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,10 +15,10 @@
     <sheet name="Página 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Página 1'!$A$1:$X$50</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Página 1'!$A$1:$X$50</definedName>
   </definedNames>
-  <calcPr calcId="171027" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1056,8 +1056,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Millares" xfId="2" builtinId="3"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1145,7 +1145,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1447,24 +1447,24 @@
   <dimension ref="A1:X50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21:M22"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="1" customWidth="1"/>
     <col min="2" max="3" width="25.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
     <col min="7" max="9" width="5.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="14.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="14" max="14" width="9.140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="24" width="7.7109375" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="25" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>